<commit_message>
0607: optimize constraint (3)
</commit_message>
<xml_diff>
--- a/BarraPCA/optimize_target_v2.xlsx
+++ b/BarraPCA/optimize_target_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\Nutstore\1\我的坚果云\XJIntern\PyCharmProject\BarraPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04E0956-DEC7-445C-8EDE-1AE97DD1625A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4677AE-07A2-46E5-9F12-7B722AA22F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>mkt_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,10 +143,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>H1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -159,19 +155,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.00</t>
+    <t>0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSI300</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -394,8 +394,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}" name="表1" displayName="表1" ref="A1:P10" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" dataCellStyle="常规">
-  <autoFilter ref="A1:P10" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}" name="表1" displayName="表1" ref="A1:P5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" dataCellStyle="常规">
+  <autoFilter ref="A1:P5" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{3AA5E9AC-0C18-4DAC-866F-47D1A8510787}" name="run" dataDxfId="15" dataCellStyle="常规"/>
     <tableColumn id="6" xr3:uid="{3D346140-5BE9-4DDD-B196-59B9BCFC3CB4}" name="alpha_name" dataDxfId="14" dataCellStyle="常规"/>
@@ -681,38 +681,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.21875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" style="1" customWidth="1"/>
+    <col min="7" max="8" width="5.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.25" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -732,10 +732,10 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>26</v>
@@ -762,9 +762,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -782,16 +782,16 @@
         <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>15</v>
@@ -812,15 +812,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
@@ -832,16 +832,16 @@
         <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>15</v>
@@ -862,7 +862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -882,16 +882,16 @@
         <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>15</v>
@@ -912,15 +912,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
@@ -935,13 +935,13 @@
         <v>24</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>15</v>
@@ -959,256 +959,6 @@
         <v>19</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0609: risk matrix cnstr
</commit_message>
<xml_diff>
--- a/BarraPCA/optimize_target_v2.xlsx
+++ b/BarraPCA/optimize_target_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\Nutstore\1\我的坚果云\XJIntern\PyCharmProject\BarraPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4677AE-07A2-46E5-9F12-7B722AA22F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B43A5F-C6F5-48EF-A99F-814E4B036413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>mkt_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>CSI300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -224,7 +236,25 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -394,25 +424,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}" name="表1" displayName="表1" ref="A1:P5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" dataCellStyle="常规">
-  <autoFilter ref="A1:P5" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{3AA5E9AC-0C18-4DAC-866F-47D1A8510787}" name="run" dataDxfId="15" dataCellStyle="常规"/>
-    <tableColumn id="6" xr3:uid="{3D346140-5BE9-4DDD-B196-59B9BCFC3CB4}" name="alpha_name" dataDxfId="14" dataCellStyle="常规"/>
-    <tableColumn id="5" xr3:uid="{D2E9FE7A-7688-4F5B-8571-57FA7F950FAC}" name="mkt_type" dataDxfId="13" dataCellStyle="常规"/>
-    <tableColumn id="7" xr3:uid="{21D2BC5B-1724-4F5A-B035-96075B1C2F09}" name="beta_kind" dataDxfId="12" dataCellStyle="常规"/>
-    <tableColumn id="15" xr3:uid="{F7C69614-6013-4F27-B374-3234DC1FBECE}" name="beta_suffix" dataDxfId="11" dataCellStyle="常规"/>
-    <tableColumn id="8" xr3:uid="{F2F7816F-F2E3-423F-878B-C3AAC4FA1D59}" name="beta_args" dataDxfId="10" dataCellStyle="常规"/>
-    <tableColumn id="2" xr3:uid="{ADC22F73-F264-4A15-91B8-8277EEDB39C1}" name="H0" dataDxfId="9" dataCellStyle="常规"/>
-    <tableColumn id="3" xr3:uid="{31851A3A-F877-49EE-AFF8-6A2B1CEA161C}" name="H1" dataDxfId="8" dataCellStyle="常规"/>
-    <tableColumn id="4" xr3:uid="{D159B152-EF17-4A53-A2B7-966C2E98AF96}" name="B" dataDxfId="7" dataCellStyle="常规"/>
-    <tableColumn id="16" xr3:uid="{C38C3F2C-D0BF-4652-9FCE-197C4FA6B9F4}" name="E" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{301040EA-8B39-49A6-93EE-2BDCD97E3D9B}" name="D" dataDxfId="5" dataCellStyle="常规"/>
-    <tableColumn id="10" xr3:uid="{6382DB46-0A90-49E0-B08D-FEC8E75AB104}" name="N" dataDxfId="4" dataCellStyle="常规"/>
-    <tableColumn id="11" xr3:uid="{DF0EDCA0-9516-45FB-BFB6-9DFB8EC0D545}" name="wei_tole" dataDxfId="3" dataCellStyle="常规"/>
-    <tableColumn id="12" xr3:uid="{60A4E7F6-72FF-4BCA-9D8F-856FA2A5D290}" name="begin_date" dataDxfId="2" dataCellStyle="常规"/>
-    <tableColumn id="13" xr3:uid="{62EA22B9-5B83-416C-B38E-2A157668E54E}" name="end_date" dataDxfId="1" dataCellStyle="常规"/>
-    <tableColumn id="14" xr3:uid="{03F4B61D-EE69-4D7C-B63A-F7ACB07450A3}" name="opt_verbose" dataDxfId="0" dataCellStyle="常规"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}" name="表1" displayName="表1" ref="A1:R5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" dataCellStyle="常规">
+  <autoFilter ref="A1:R5" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{3AA5E9AC-0C18-4DAC-866F-47D1A8510787}" name="run" dataDxfId="17" dataCellStyle="常规"/>
+    <tableColumn id="6" xr3:uid="{3D346140-5BE9-4DDD-B196-59B9BCFC3CB4}" name="alpha_name" dataDxfId="16" dataCellStyle="常规"/>
+    <tableColumn id="5" xr3:uid="{D2E9FE7A-7688-4F5B-8571-57FA7F950FAC}" name="mkt_type" dataDxfId="15" dataCellStyle="常规"/>
+    <tableColumn id="7" xr3:uid="{21D2BC5B-1724-4F5A-B035-96075B1C2F09}" name="beta_kind" dataDxfId="14" dataCellStyle="常规"/>
+    <tableColumn id="15" xr3:uid="{F7C69614-6013-4F27-B374-3234DC1FBECE}" name="beta_suffix" dataDxfId="13" dataCellStyle="常规"/>
+    <tableColumn id="8" xr3:uid="{F2F7816F-F2E3-423F-878B-C3AAC4FA1D59}" name="beta_args" dataDxfId="12" dataCellStyle="常规"/>
+    <tableColumn id="2" xr3:uid="{ADC22F73-F264-4A15-91B8-8277EEDB39C1}" name="H0" dataDxfId="11" dataCellStyle="常规"/>
+    <tableColumn id="3" xr3:uid="{31851A3A-F877-49EE-AFF8-6A2B1CEA161C}" name="H1" dataDxfId="10" dataCellStyle="常规"/>
+    <tableColumn id="4" xr3:uid="{D159B152-EF17-4A53-A2B7-966C2E98AF96}" name="B" dataDxfId="9" dataCellStyle="常规"/>
+    <tableColumn id="16" xr3:uid="{C38C3F2C-D0BF-4652-9FCE-197C4FA6B9F4}" name="E" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{301040EA-8B39-49A6-93EE-2BDCD97E3D9B}" name="D" dataDxfId="7" dataCellStyle="常规"/>
+    <tableColumn id="17" xr3:uid="{530D8216-A88C-4A03-8B8B-6CDB5325F543}" name="G" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{E7F1B0A8-266A-461F-8997-857270CD3CEF}" name="S" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{6382DB46-0A90-49E0-B08D-FEC8E75AB104}" name="N" dataDxfId="6" dataCellStyle="常规"/>
+    <tableColumn id="11" xr3:uid="{DF0EDCA0-9516-45FB-BFB6-9DFB8EC0D545}" name="wei_tole" dataDxfId="5" dataCellStyle="常规"/>
+    <tableColumn id="12" xr3:uid="{60A4E7F6-72FF-4BCA-9D8F-856FA2A5D290}" name="begin_date" dataDxfId="4" dataCellStyle="常规"/>
+    <tableColumn id="13" xr3:uid="{62EA22B9-5B83-416C-B38E-2A157668E54E}" name="end_date" dataDxfId="3" dataCellStyle="常规"/>
+    <tableColumn id="14" xr3:uid="{03F4B61D-EE69-4D7C-B63A-F7ACB07450A3}" name="opt_verbose" dataDxfId="2" dataCellStyle="常规"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -681,38 +713,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" style="1" customWidth="1"/>
-    <col min="7" max="8" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.25" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.125" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.875" style="1"/>
+    <col min="1" max="1" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.21875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.109375" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -747,22 +781,28 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -797,22 +837,28 @@
         <v>15</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -847,22 +893,28 @@
         <v>15</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -897,22 +949,28 @@
         <v>15</v>
       </c>
       <c r="L4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -947,18 +1005,24 @@
         <v>15</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
argparse example & optimize with G
</commit_message>
<xml_diff>
--- a/BarraPCA/optimize_target_v2.xlsx
+++ b/BarraPCA/optimize_target_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\Nutstore\1\我的坚果云\XJIntern\PyCharmProject\BarraPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B43A5F-C6F5-48EF-A99F-814E4B036413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1785065-46B5-4777-AFDE-F6216AC52284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="38">
   <si>
     <t>mkt_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -183,7 +183,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.1</t>
+    <t>2.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -424,8 +424,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}" name="表1" displayName="表1" ref="A1:R5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" dataCellStyle="常规">
-  <autoFilter ref="A1:R5" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}" name="表1" displayName="表1" ref="A1:R13" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" dataCellStyle="常规">
+  <autoFilter ref="A1:R13" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{3AA5E9AC-0C18-4DAC-866F-47D1A8510787}" name="run" dataDxfId="17" dataCellStyle="常规"/>
     <tableColumn id="6" xr3:uid="{3D346140-5BE9-4DDD-B196-59B9BCFC3CB4}" name="alpha_name" dataDxfId="16" dataCellStyle="常规"/>
@@ -438,13 +438,13 @@
     <tableColumn id="4" xr3:uid="{D159B152-EF17-4A53-A2B7-966C2E98AF96}" name="B" dataDxfId="9" dataCellStyle="常规"/>
     <tableColumn id="16" xr3:uid="{C38C3F2C-D0BF-4652-9FCE-197C4FA6B9F4}" name="E" dataDxfId="8"/>
     <tableColumn id="9" xr3:uid="{301040EA-8B39-49A6-93EE-2BDCD97E3D9B}" name="D" dataDxfId="7" dataCellStyle="常规"/>
-    <tableColumn id="17" xr3:uid="{530D8216-A88C-4A03-8B8B-6CDB5325F543}" name="G" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{E7F1B0A8-266A-461F-8997-857270CD3CEF}" name="S" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{6382DB46-0A90-49E0-B08D-FEC8E75AB104}" name="N" dataDxfId="6" dataCellStyle="常规"/>
-    <tableColumn id="11" xr3:uid="{DF0EDCA0-9516-45FB-BFB6-9DFB8EC0D545}" name="wei_tole" dataDxfId="5" dataCellStyle="常规"/>
-    <tableColumn id="12" xr3:uid="{60A4E7F6-72FF-4BCA-9D8F-856FA2A5D290}" name="begin_date" dataDxfId="4" dataCellStyle="常规"/>
-    <tableColumn id="13" xr3:uid="{62EA22B9-5B83-416C-B38E-2A157668E54E}" name="end_date" dataDxfId="3" dataCellStyle="常规"/>
-    <tableColumn id="14" xr3:uid="{03F4B61D-EE69-4D7C-B63A-F7ACB07450A3}" name="opt_verbose" dataDxfId="2" dataCellStyle="常规"/>
+    <tableColumn id="17" xr3:uid="{530D8216-A88C-4A03-8B8B-6CDB5325F543}" name="G" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{E7F1B0A8-266A-461F-8997-857270CD3CEF}" name="S" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{6382DB46-0A90-49E0-B08D-FEC8E75AB104}" name="N" dataDxfId="4" dataCellStyle="常规"/>
+    <tableColumn id="11" xr3:uid="{DF0EDCA0-9516-45FB-BFB6-9DFB8EC0D545}" name="wei_tole" dataDxfId="3" dataCellStyle="常规"/>
+    <tableColumn id="12" xr3:uid="{60A4E7F6-72FF-4BCA-9D8F-856FA2A5D290}" name="begin_date" dataDxfId="2" dataCellStyle="常规"/>
+    <tableColumn id="13" xr3:uid="{62EA22B9-5B83-416C-B38E-2A157668E54E}" name="end_date" dataDxfId="1" dataCellStyle="常规"/>
+    <tableColumn id="14" xr3:uid="{03F4B61D-EE69-4D7C-B63A-F7ACB07450A3}" name="opt_verbose" dataDxfId="0" dataCellStyle="常规"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -713,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -726,11 +726,11 @@
     <col min="4" max="4" width="11.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.88671875" style="1" customWidth="1"/>
     <col min="14" max="14" width="6.44140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="1" bestFit="1" customWidth="1"/>
@@ -804,7 +804,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -1023,6 +1023,454 @@
         <v>19</v>
       </c>
       <c r="R5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimize: manually shift fct_cov, stk_rsk, todo
</commit_message>
<xml_diff>
--- a/BarraPCA/optimize_target_v2.xlsx
+++ b/BarraPCA/optimize_target_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\Nutstore\1\我的坚果云\XJIntern\PyCharmProject\BarraPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1785065-46B5-4777-AFDE-F6216AC52284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69280B93-D702-4981-BE98-8804F03CAB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -716,12 +716,13 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -804,7 +805,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -860,7 +861,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -916,7 +917,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -972,7 +973,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
optimize: skip existed res in multi-process
</commit_message>
<xml_diff>
--- a/BarraPCA/optimize_target_v2.xlsx
+++ b/BarraPCA/optimize_target_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\Nutstore\1\我的坚果云\XJIntern\PyCharmProject\BarraPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD19D11-E750-40D2-8DEE-A58F5C1FDB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A077CA87-42B4-4A11-961F-251DF08F91A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2928" yWindow="3000" windowWidth="20112" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="40">
   <si>
     <t>mkt_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -167,15 +167,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSI500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>CSI300</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -416,8 +432,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}" name="表1" displayName="表1" ref="A1:R5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" dataCellStyle="常规">
-  <autoFilter ref="A1:R5" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}" name="表1" displayName="表1" ref="A1:R21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" dataCellStyle="常规">
+  <autoFilter ref="A1:R21" xr:uid="{1CC0EBF8-895C-4A90-B8C4-BCEE32DB2B69}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{3AA5E9AC-0C18-4DAC-866F-47D1A8510787}" name="run" dataDxfId="17" dataCellStyle="常规"/>
     <tableColumn id="6" xr3:uid="{3D346140-5BE9-4DDD-B196-59B9BCFC3CB4}" name="alpha_name" dataDxfId="16" dataCellStyle="常规"/>
@@ -705,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C12" sqref="C12:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -802,7 +818,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -829,7 +845,7 @@
         <v>13</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>14</v>
@@ -858,7 +874,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -885,7 +901,7 @@
         <v>13</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>14</v>
@@ -914,7 +930,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -938,10 +954,10 @@
         <v>34</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>14</v>
@@ -970,7 +986,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -994,10 +1010,10 @@
         <v>34</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>14</v>
@@ -1015,6 +1031,902 @@
         <v>17</v>
       </c>
       <c r="R5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>